<commit_message>
Primera versión de mapas
</commit_message>
<xml_diff>
--- a/Inputs/descarga_original.xlsx
+++ b/Inputs/descarga_original.xlsx
@@ -2319,10 +2319,12 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2576,9 +2578,9 @@
       <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="135" width="21.57"/>
+    <col customWidth="1" min="1" max="135" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
mejoras en los mapas
</commit_message>
<xml_diff>
--- a/Inputs/descarga_original.xlsx
+++ b/Inputs/descarga_original.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$CU$70</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$CU$72</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5959" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6129" uniqueCount="832">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -2479,6 +2479,36 @@
   </si>
   <si>
     <t xml:space="preserve">Difícil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cocinar </t>
+  </si>
+  <si>
+    <t>Cocina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emplatar viandas </t>
+  </si>
+  <si>
+    <t>Primer Cuatrimestre</t>
+  </si>
+  <si>
+    <t>miayeve2017@gmail.com</t>
+  </si>
+  <si>
+    <t>Rodolfo walsh</t>
+  </si>
+  <si>
+    <t>Administrativa medica</t>
+  </si>
+  <si>
+    <t>Recepcion de pacientes, armado de hc, asignacion de turnos y preparar los co sultorios de los medicos</t>
+  </si>
+  <si>
+    <t>Comparacion</t>
+  </si>
+  <si>
+    <t>MICAELA, VERDES</t>
   </si>
 </sst>
 </file>
@@ -2520,7 +2550,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2542,6 +2572,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -25830,10 +25863,650 @@
       <c r="DV70" s="7"/>
     </row>
     <row r="71">
-      <c r="E71" s="2"/>
+      <c r="A71" s="4">
+        <v>44655.3699775</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E71" s="9">
+        <v>33769.0</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G71" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J71" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="M71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="P71" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q71" s="3">
+        <v>1208.0</v>
+      </c>
+      <c r="R71" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="S71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="U71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="V71" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="W71" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="X71" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y71" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z71" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA71" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="AB71" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="AC71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE71" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF71" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG71" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH71" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="AI71" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="AJ71" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="AK71" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="AL71" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="AM71" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="AN71" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="AO71" s="3">
+        <v>7500.0</v>
+      </c>
+      <c r="AP71" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ71" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR71" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="AS71" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AT71" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AU71" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AV71" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AW71" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AX71" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="AY71" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AZ71" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA71" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB71" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="BC71" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="BD71" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE71" s="3">
+        <v>2019.0</v>
+      </c>
+      <c r="BF71" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="BG71" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="BH71" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="BI71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="BJ71" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="BK71" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="BL71" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="BM71" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="BN71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="BO71" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="BP71" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="BQ71" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BR71" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="BS71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="BV71" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="BW71" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="BX71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="BY71" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="BZ71" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="CA71" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="CB71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CC71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CD71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CE71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CF71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CG71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CH71" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="CI71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CJ71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CK71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CL71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CM71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CN71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CO71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CP71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CQ71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CR71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CS71" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="CT71" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="CU71" s="3">
+        <v>3.6761296E7</v>
+      </c>
+      <c r="CW71" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="CX71" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="CY71" s="3">
+        <v>2022.0</v>
+      </c>
+      <c r="CZ71" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="DA71" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="DB71" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="DC71" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="DD71" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="DE71" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="DF71" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="DG71" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="DH71" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="DI71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="DJ71" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="DK71" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="DL71" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="DM71" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="DN71" s="3" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="72">
-      <c r="E72" s="2"/>
+      <c r="A72" s="4">
+        <v>44655.49384729167</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>826</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E72" s="9">
+        <v>33859.0</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G72" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J72" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="M72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="P72" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="Q72" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="R72" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="S72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="T72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="U72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="V72" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="W72" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="X72" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y72" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="Z72" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA72" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="AB72" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="AC72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE72" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF72" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG72" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH72" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="AI72" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="AJ72" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="AK72" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="AL72" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="AM72" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="AN72" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="AO72" s="3">
+        <v>7500.0</v>
+      </c>
+      <c r="AP72" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AQ72" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AR72" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AS72" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AT72" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AU72" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV72" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="AW72" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="AX72" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AY72" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AZ72" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="BA72" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="BB72" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="BC72" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="BD72" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE72" s="3">
+        <v>2021.0</v>
+      </c>
+      <c r="BF72" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="BG72" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="BH72" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="BI72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="BJ72" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="BK72" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="BL72" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="BM72" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="BN72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="BO72" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="BP72" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="BQ72" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="BS72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="BT72" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="BU72" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="CI72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CJ72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CK72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CL72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CM72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CN72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CO72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CP72" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CQ72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CR72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CS72" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="CT72" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="CU72" s="3">
+        <v>3.7085431E7</v>
+      </c>
+      <c r="CW72" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="CX72" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="CY72" s="3">
+        <v>2022.0</v>
+      </c>
+      <c r="CZ72" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="DA72" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="DB72" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="DC72" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="DD72" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="DE72" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="DF72" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="DG72" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="DH72" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="DI72" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="DJ72" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="DK72" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="DL72" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="DM72" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="DN72" s="3" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="73">
       <c r="E73" s="2"/>
@@ -26129,8 +26802,14 @@
     <row r="170">
       <c r="E170" s="2"/>
     </row>
+    <row r="171">
+      <c r="E171" s="2"/>
+    </row>
+    <row r="172">
+      <c r="E172" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$CU$70"/>
+  <autoFilter ref="$A$1:$CU$72"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>